<commit_message>
Right format of longitude and latitide
</commit_message>
<xml_diff>
--- a/resources/excel/magenta.xlsx
+++ b/resources/excel/magenta.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\codeweek\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90A480F0-CBDF-4C17-86D2-126DB8E71B8E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF20ECA3-4B28-403E-8C6C-4374C9F75A76}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="26790" yWindow="2190" windowWidth="23505" windowHeight="16290" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -291,6 +291,12 @@
     <t>Type of Organization</t>
   </si>
   <si>
+    <t>52.5103735</t>
+  </si>
+  <si>
+    <t>13.3761809</t>
+  </si>
+  <si>
     <t>https://codeweek-s3.s3-eu-west-1.amazonaws.com/events/pictures/magenta/2.png</t>
   </si>
   <si>
@@ -322,12 +328,6 @@
   </si>
   <si>
     <t>https://codeweek-s3.s3-eu-west-1.amazonaws.com/events/pictures/magenta/3.png</t>
-  </si>
-  <si>
-    <t>13,3761809</t>
-  </si>
-  <si>
-    <t>52,5103735</t>
   </si>
 </sst>
 </file>
@@ -786,8 +786,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:R139"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="P4" sqref="P4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="50.1" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -910,13 +910,13 @@
         <v>22</v>
       </c>
       <c r="O2" s="14" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="P2" s="14" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="Q2" s="7" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="R2">
         <v>157182</v>
@@ -966,13 +966,13 @@
         <v>22</v>
       </c>
       <c r="O3" s="14" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="P3" s="14" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="Q3" s="7" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="R3">
         <v>157182</v>
@@ -1022,13 +1022,13 @@
         <v>22</v>
       </c>
       <c r="O4" s="14" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="P4" s="14" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="Q4" s="7" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="R4">
         <v>157182</v>
@@ -1078,13 +1078,13 @@
         <v>22</v>
       </c>
       <c r="O5" s="14" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="P5" s="14" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="Q5" s="7" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="R5">
         <v>157182</v>
@@ -1134,13 +1134,13 @@
         <v>22</v>
       </c>
       <c r="O6" s="14" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="P6" s="14" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="Q6" s="7" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="R6">
         <v>157182</v>
@@ -1190,13 +1190,13 @@
         <v>22</v>
       </c>
       <c r="O7" s="14" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="P7" s="14" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="Q7" s="7" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="R7">
         <v>157182</v>
@@ -1246,13 +1246,13 @@
         <v>22</v>
       </c>
       <c r="O8" s="14" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="P8" s="14" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="Q8" s="7" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="R8">
         <v>157182</v>
@@ -1302,13 +1302,13 @@
         <v>22</v>
       </c>
       <c r="O9" s="14" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="P9" s="14" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="Q9" s="7" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="R9">
         <v>157182</v>
@@ -1358,13 +1358,13 @@
         <v>22</v>
       </c>
       <c r="O10" s="14" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="P10" s="14" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="Q10" s="7" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="R10">
         <v>157182</v>
@@ -1414,13 +1414,13 @@
         <v>22</v>
       </c>
       <c r="O11" s="14" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="P11" s="14" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="Q11" s="7" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="R11">
         <v>157182</v>
@@ -1470,13 +1470,13 @@
         <v>22</v>
       </c>
       <c r="O12" s="14" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="P12" s="14" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="Q12" s="7" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="R12">
         <v>157182</v>
@@ -1526,13 +1526,13 @@
         <v>22</v>
       </c>
       <c r="O13" s="14" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="P13" s="14" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="Q13" s="7" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="R13">
         <v>157182</v>
@@ -1582,13 +1582,13 @@
         <v>22</v>
       </c>
       <c r="O14" s="14" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="P14" s="14" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="Q14" s="7" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="R14">
         <v>157182</v>
@@ -1638,13 +1638,13 @@
         <v>22</v>
       </c>
       <c r="O15" s="14" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="P15" s="14" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="Q15" s="7" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="R15">
         <v>157182</v>
@@ -1694,13 +1694,13 @@
         <v>22</v>
       </c>
       <c r="O16" s="14" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="P16" s="14" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="Q16" s="7" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="R16">
         <v>157182</v>
@@ -1750,13 +1750,13 @@
         <v>22</v>
       </c>
       <c r="O17" s="14" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="P17" s="14" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="Q17" s="7" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="R17">
         <v>157182</v>
@@ -1806,13 +1806,13 @@
         <v>22</v>
       </c>
       <c r="O18" s="14" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="P18" s="14" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="Q18" s="7" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="R18">
         <v>157182</v>
@@ -1862,13 +1862,13 @@
         <v>22</v>
       </c>
       <c r="O19" s="14" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="P19" s="14" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="Q19" s="7" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="R19">
         <v>157182</v>
@@ -1918,13 +1918,13 @@
         <v>22</v>
       </c>
       <c r="O20" s="14" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="P20" s="14" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="Q20" s="7" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="R20">
         <v>157182</v>
@@ -1974,13 +1974,13 @@
         <v>22</v>
       </c>
       <c r="O21" s="14" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="P21" s="14" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="Q21" s="7" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="R21">
         <v>157182</v>
@@ -2030,13 +2030,13 @@
         <v>22</v>
       </c>
       <c r="O22" s="14" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="P22" s="14" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="Q22" s="7" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="R22">
         <v>157182</v>
@@ -2086,13 +2086,13 @@
         <v>22</v>
       </c>
       <c r="O23" s="14" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="P23" s="14" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="Q23" s="7" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="R23">
         <v>157182</v>
@@ -2142,13 +2142,13 @@
         <v>22</v>
       </c>
       <c r="O24" s="14" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="P24" s="14" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="Q24" s="7" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="R24">
         <v>157182</v>
@@ -2198,13 +2198,13 @@
         <v>22</v>
       </c>
       <c r="O25" s="14" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="P25" s="14" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="Q25" s="7" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="R25">
         <v>157182</v>
@@ -2254,13 +2254,13 @@
         <v>22</v>
       </c>
       <c r="O26" s="14" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="P26" s="14" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="Q26" s="7" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="R26">
         <v>157182</v>
@@ -2310,13 +2310,13 @@
         <v>22</v>
       </c>
       <c r="O27" s="14" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="P27" s="14" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="Q27" s="7" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="R27">
         <v>157182</v>
@@ -2366,13 +2366,13 @@
         <v>22</v>
       </c>
       <c r="O28" s="14" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="P28" s="14" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="Q28" s="7" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="R28">
         <v>157182</v>
@@ -2422,13 +2422,13 @@
         <v>22</v>
       </c>
       <c r="O29" s="14" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="P29" s="14" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="Q29" s="7" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="R29">
         <v>157182</v>
@@ -2478,13 +2478,13 @@
         <v>22</v>
       </c>
       <c r="O30" s="14" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="P30" s="14" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="Q30" s="7" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="R30">
         <v>157182</v>
@@ -2534,13 +2534,13 @@
         <v>22</v>
       </c>
       <c r="O31" s="14" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="P31" s="14" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="Q31" s="7" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="R31">
         <v>157182</v>
@@ -2590,13 +2590,13 @@
         <v>22</v>
       </c>
       <c r="O32" s="14" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="P32" s="14" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="Q32" s="7" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="R32">
         <v>157182</v>
@@ -2646,13 +2646,13 @@
         <v>22</v>
       </c>
       <c r="O33" s="14" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="P33" s="14" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="Q33" s="7" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="R33">
         <v>157182</v>
@@ -2702,13 +2702,13 @@
         <v>22</v>
       </c>
       <c r="O34" s="14" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="P34" s="14" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="Q34" s="7" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="R34">
         <v>157182</v>
@@ -2758,13 +2758,13 @@
         <v>22</v>
       </c>
       <c r="O35" s="14" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="P35" s="14" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="Q35" s="7" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="R35">
         <v>157182</v>
@@ -2814,13 +2814,13 @@
         <v>22</v>
       </c>
       <c r="O36" s="14" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="P36" s="14" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="Q36" s="7" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="R36">
         <v>157182</v>
@@ -2870,13 +2870,13 @@
         <v>22</v>
       </c>
       <c r="O37" s="14" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="P37" s="14" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="Q37" s="7" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="R37">
         <v>157182</v>
@@ -2926,13 +2926,13 @@
         <v>22</v>
       </c>
       <c r="O38" s="14" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="P38" s="14" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="Q38" s="7" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="R38">
         <v>157182</v>
@@ -2982,13 +2982,13 @@
         <v>22</v>
       </c>
       <c r="O39" s="14" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="P39" s="14" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="Q39" s="7" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="R39">
         <v>157182</v>
@@ -3038,13 +3038,13 @@
         <v>22</v>
       </c>
       <c r="O40" s="14" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="P40" s="14" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="Q40" s="7" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="R40">
         <v>157182</v>
@@ -3094,13 +3094,13 @@
         <v>22</v>
       </c>
       <c r="O41" s="14" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="P41" s="14" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="Q41" s="7" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="R41">
         <v>157182</v>
@@ -3150,13 +3150,13 @@
         <v>22</v>
       </c>
       <c r="O42" s="14" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="P42" s="14" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="Q42" s="7" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="R42">
         <v>157182</v>
@@ -3206,13 +3206,13 @@
         <v>22</v>
       </c>
       <c r="O43" s="14" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="P43" s="14" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="Q43" s="7" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="R43">
         <v>157182</v>
@@ -3262,13 +3262,13 @@
         <v>22</v>
       </c>
       <c r="O44" s="14" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="P44" s="14" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="Q44" s="7" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="R44">
         <v>157182</v>
@@ -3318,13 +3318,13 @@
         <v>22</v>
       </c>
       <c r="O45" s="14" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="P45" s="14" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="Q45" s="7" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="R45">
         <v>157182</v>
@@ -3374,13 +3374,13 @@
         <v>22</v>
       </c>
       <c r="O46" s="14" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="P46" s="14" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="Q46" s="7" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="R46">
         <v>157182</v>
@@ -3430,13 +3430,13 @@
         <v>22</v>
       </c>
       <c r="O47" s="14" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="P47" s="14" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="Q47" s="7" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="R47">
         <v>157182</v>
@@ -3486,13 +3486,13 @@
         <v>22</v>
       </c>
       <c r="O48" s="14" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="P48" s="14" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="Q48" s="7" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="R48">
         <v>157182</v>
@@ -3542,13 +3542,13 @@
         <v>22</v>
       </c>
       <c r="O49" s="14" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="P49" s="14" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="Q49" s="7" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="R49">
         <v>157182</v>
@@ -3598,13 +3598,13 @@
         <v>22</v>
       </c>
       <c r="O50" s="14" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="P50" s="14" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="Q50" s="7" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="R50">
         <v>157182</v>
@@ -3654,13 +3654,13 @@
         <v>22</v>
       </c>
       <c r="O51" s="14" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="P51" s="14" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="Q51" s="7" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="R51">
         <v>157182</v>
@@ -3710,13 +3710,13 @@
         <v>22</v>
       </c>
       <c r="O52" s="14" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="P52" s="14" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="Q52" s="7" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="R52">
         <v>157182</v>
@@ -3766,13 +3766,13 @@
         <v>22</v>
       </c>
       <c r="O53" s="14" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="P53" s="14" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="Q53" s="7" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="R53">
         <v>157182</v>
@@ -3822,13 +3822,13 @@
         <v>22</v>
       </c>
       <c r="O54" s="14" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="P54" s="14" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="Q54" s="7" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="R54">
         <v>157182</v>
@@ -3878,13 +3878,13 @@
         <v>22</v>
       </c>
       <c r="O55" s="14" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="P55" s="14" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="Q55" s="7" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="R55">
         <v>157182</v>
@@ -3934,13 +3934,13 @@
         <v>22</v>
       </c>
       <c r="O56" s="14" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="P56" s="14" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="Q56" s="7" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="R56">
         <v>157182</v>
@@ -3990,13 +3990,13 @@
         <v>22</v>
       </c>
       <c r="O57" s="14" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="P57" s="14" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="Q57" s="7" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="R57">
         <v>157182</v>
@@ -4046,13 +4046,13 @@
         <v>22</v>
       </c>
       <c r="O58" s="14" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="P58" s="14" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="Q58" s="7" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="R58">
         <v>157182</v>
@@ -4102,13 +4102,13 @@
         <v>22</v>
       </c>
       <c r="O59" s="14" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="P59" s="14" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="Q59" s="7" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="R59">
         <v>157182</v>
@@ -4158,13 +4158,13 @@
         <v>22</v>
       </c>
       <c r="O60" s="14" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="P60" s="14" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="Q60" s="7" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="R60">
         <v>157182</v>
@@ -4214,13 +4214,13 @@
         <v>22</v>
       </c>
       <c r="O61" s="14" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="P61" s="14" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="Q61" s="7" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="R61">
         <v>157182</v>
@@ -4270,13 +4270,13 @@
         <v>22</v>
       </c>
       <c r="O62" s="14" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="P62" s="14" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="Q62" s="7" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="R62">
         <v>157182</v>
@@ -4326,13 +4326,13 @@
         <v>22</v>
       </c>
       <c r="O63" s="14" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="P63" s="14" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="Q63" s="7" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="R63">
         <v>157182</v>
@@ -4382,13 +4382,13 @@
         <v>22</v>
       </c>
       <c r="O64" s="14" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="P64" s="14" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="Q64" s="7" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="R64">
         <v>157182</v>
@@ -4438,13 +4438,13 @@
         <v>22</v>
       </c>
       <c r="O65" s="14" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="P65" s="14" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="Q65" s="7" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="R65">
         <v>157182</v>
@@ -4494,13 +4494,13 @@
         <v>22</v>
       </c>
       <c r="O66" s="14" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="P66" s="14" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="Q66" s="7" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="R66">
         <v>157182</v>
@@ -4550,13 +4550,13 @@
         <v>22</v>
       </c>
       <c r="O67" s="14" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="P67" s="14" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="Q67" s="7" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="R67">
         <v>157182</v>
@@ -4606,13 +4606,13 @@
         <v>22</v>
       </c>
       <c r="O68" s="14" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="P68" s="14" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="Q68" s="7" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="R68">
         <v>157182</v>
@@ -4662,13 +4662,13 @@
         <v>22</v>
       </c>
       <c r="O69" s="14" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="P69" s="14" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="Q69" s="7" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="R69">
         <v>157182</v>
@@ -4718,13 +4718,13 @@
         <v>22</v>
       </c>
       <c r="O70" s="14" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="P70" s="14" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="Q70" s="7" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="R70">
         <v>157182</v>
@@ -4774,13 +4774,13 @@
         <v>22</v>
       </c>
       <c r="O71" s="14" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="P71" s="14" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="Q71" s="7" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="R71">
         <v>157182</v>
@@ -4830,13 +4830,13 @@
         <v>22</v>
       </c>
       <c r="O72" s="14" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="P72" s="14" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="Q72" s="7" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="R72">
         <v>157182</v>
@@ -4886,13 +4886,13 @@
         <v>22</v>
       </c>
       <c r="O73" s="14" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="P73" s="14" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="Q73" s="7" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="R73">
         <v>157182</v>
@@ -4942,13 +4942,13 @@
         <v>22</v>
       </c>
       <c r="O74" s="14" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="P74" s="14" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="Q74" s="7" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="R74">
         <v>157182</v>
@@ -4998,13 +4998,13 @@
         <v>22</v>
       </c>
       <c r="O75" s="14" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="P75" s="14" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="Q75" s="7" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="R75">
         <v>157182</v>
@@ -5054,13 +5054,13 @@
         <v>22</v>
       </c>
       <c r="O76" s="14" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="P76" s="14" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="Q76" s="7" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="R76">
         <v>157182</v>
@@ -5110,13 +5110,13 @@
         <v>22</v>
       </c>
       <c r="O77" s="14" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="P77" s="14" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="Q77" s="7" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="R77">
         <v>157182</v>
@@ -5166,13 +5166,13 @@
         <v>22</v>
       </c>
       <c r="O78" s="14" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="P78" s="14" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="Q78" s="7" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="R78">
         <v>157182</v>
@@ -5222,13 +5222,13 @@
         <v>22</v>
       </c>
       <c r="O79" s="14" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="P79" s="14" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="Q79" s="7" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="R79">
         <v>157182</v>
@@ -5278,13 +5278,13 @@
         <v>22</v>
       </c>
       <c r="O80" s="14" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="P80" s="14" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="Q80" s="7" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="R80">
         <v>157182</v>
@@ -5334,13 +5334,13 @@
         <v>22</v>
       </c>
       <c r="O81" s="14" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="P81" s="14" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="Q81" s="7" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="R81">
         <v>157182</v>
@@ -5390,13 +5390,13 @@
         <v>22</v>
       </c>
       <c r="O82" s="14" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="P82" s="14" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="Q82" s="7" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="R82">
         <v>157182</v>
@@ -5446,13 +5446,13 @@
         <v>22</v>
       </c>
       <c r="O83" s="14" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="P83" s="14" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="Q83" s="7" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="R83">
         <v>157182</v>
@@ -5502,13 +5502,13 @@
         <v>22</v>
       </c>
       <c r="O84" s="14" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="P84" s="14" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="Q84" s="7" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="R84">
         <v>157182</v>
@@ -5558,13 +5558,13 @@
         <v>22</v>
       </c>
       <c r="O85" s="14" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="P85" s="14" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="Q85" s="7" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="R85">
         <v>157182</v>
@@ -5614,13 +5614,13 @@
         <v>22</v>
       </c>
       <c r="O86" s="14" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="P86" s="14" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="Q86" s="7" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="R86">
         <v>157182</v>
@@ -5670,13 +5670,13 @@
         <v>22</v>
       </c>
       <c r="O87" s="14" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="P87" s="14" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="Q87" s="7" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="R87">
         <v>157182</v>
@@ -5726,13 +5726,13 @@
         <v>22</v>
       </c>
       <c r="O88" s="14" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="P88" s="14" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="Q88" s="7" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="R88">
         <v>157182</v>
@@ -5782,13 +5782,13 @@
         <v>22</v>
       </c>
       <c r="O89" s="14" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="P89" s="14" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="Q89" s="7" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="R89">
         <v>157182</v>
@@ -5838,13 +5838,13 @@
         <v>22</v>
       </c>
       <c r="O90" s="14" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="P90" s="14" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="Q90" s="7" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="R90">
         <v>157182</v>
@@ -5894,13 +5894,13 @@
         <v>22</v>
       </c>
       <c r="O91" s="14" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="P91" s="14" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="Q91" s="7" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="R91">
         <v>157182</v>
@@ -5950,13 +5950,13 @@
         <v>22</v>
       </c>
       <c r="O92" s="14" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="P92" s="14" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="Q92" s="7" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="R92">
         <v>157182</v>
@@ -6006,13 +6006,13 @@
         <v>22</v>
       </c>
       <c r="O93" s="14" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="P93" s="14" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="Q93" s="7" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="R93">
         <v>157182</v>
@@ -6062,13 +6062,13 @@
         <v>22</v>
       </c>
       <c r="O94" s="14" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="P94" s="14" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="Q94" s="7" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="R94">
         <v>157182</v>
@@ -6118,13 +6118,13 @@
         <v>22</v>
       </c>
       <c r="O95" s="14" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="P95" s="14" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="Q95" s="7" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="R95">
         <v>157182</v>
@@ -6174,13 +6174,13 @@
         <v>22</v>
       </c>
       <c r="O96" s="14" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="P96" s="14" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="Q96" s="7" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="R96">
         <v>157182</v>
@@ -6230,13 +6230,13 @@
         <v>22</v>
       </c>
       <c r="O97" s="14" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="P97" s="14" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="Q97" s="7" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="R97">
         <v>157182</v>
@@ -6286,13 +6286,13 @@
         <v>22</v>
       </c>
       <c r="O98" s="14" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="P98" s="14" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="Q98" s="7" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="R98">
         <v>157182</v>
@@ -6342,13 +6342,13 @@
         <v>22</v>
       </c>
       <c r="O99" s="14" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="P99" s="14" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="Q99" s="7" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="R99">
         <v>157182</v>
@@ -6398,13 +6398,13 @@
         <v>22</v>
       </c>
       <c r="O100" s="14" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="P100" s="14" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="Q100" s="7" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="R100">
         <v>157182</v>
@@ -6454,13 +6454,13 @@
         <v>22</v>
       </c>
       <c r="O101" s="14" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="P101" s="14" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="Q101" s="7" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="R101">
         <v>157182</v>
@@ -6510,13 +6510,13 @@
         <v>22</v>
       </c>
       <c r="O102" s="14" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="P102" s="14" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="Q102" s="7" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="R102">
         <v>157182</v>
@@ -6566,13 +6566,13 @@
         <v>22</v>
       </c>
       <c r="O103" s="14" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="P103" s="14" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="Q103" s="7" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="R103">
         <v>157182</v>
@@ -6622,13 +6622,13 @@
         <v>22</v>
       </c>
       <c r="O104" s="14" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="P104" s="14" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="Q104" s="7" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="R104">
         <v>157182</v>
@@ -6678,13 +6678,13 @@
         <v>22</v>
       </c>
       <c r="O105" s="14" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="P105" s="14" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="Q105" s="7" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="R105">
         <v>157182</v>
@@ -6734,13 +6734,13 @@
         <v>22</v>
       </c>
       <c r="O106" s="14" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="P106" s="14" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="Q106" s="7" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="R106">
         <v>157182</v>
@@ -6790,13 +6790,13 @@
         <v>22</v>
       </c>
       <c r="O107" s="14" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="P107" s="14" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="Q107" s="7" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="R107">
         <v>157182</v>
@@ -6846,13 +6846,13 @@
         <v>22</v>
       </c>
       <c r="O108" s="14" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="P108" s="14" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="Q108" s="7" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="R108">
         <v>157182</v>
@@ -6902,13 +6902,13 @@
         <v>22</v>
       </c>
       <c r="O109" s="14" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="P109" s="14" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="Q109" s="7" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="R109">
         <v>157182</v>
@@ -6958,13 +6958,13 @@
         <v>22</v>
       </c>
       <c r="O110" s="14" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="P110" s="14" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="Q110" s="7" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="R110">
         <v>157182</v>
@@ -7014,13 +7014,13 @@
         <v>22</v>
       </c>
       <c r="O111" s="14" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="P111" s="14" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="Q111" s="7" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="R111">
         <v>157182</v>
@@ -7070,13 +7070,13 @@
         <v>22</v>
       </c>
       <c r="O112" s="14" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="P112" s="14" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="Q112" s="7" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="R112">
         <v>157182</v>
@@ -7126,13 +7126,13 @@
         <v>22</v>
       </c>
       <c r="O113" s="14" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="P113" s="14" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="Q113" s="7" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="R113">
         <v>157182</v>
@@ -7182,13 +7182,13 @@
         <v>22</v>
       </c>
       <c r="O114" s="14" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="P114" s="14" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="Q114" s="7" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="R114">
         <v>157182</v>
@@ -7238,13 +7238,13 @@
         <v>22</v>
       </c>
       <c r="O115" s="14" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="P115" s="14" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="Q115" s="7" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="R115">
         <v>157182</v>
@@ -7294,13 +7294,13 @@
         <v>22</v>
       </c>
       <c r="O116" s="14" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="P116" s="14" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="Q116" s="7" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="R116">
         <v>157182</v>
@@ -7350,13 +7350,13 @@
         <v>22</v>
       </c>
       <c r="O117" s="14" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="P117" s="14" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="Q117" s="7" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="R117">
         <v>157182</v>
@@ -7406,13 +7406,13 @@
         <v>22</v>
       </c>
       <c r="O118" s="14" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="P118" s="14" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="Q118" s="7" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="R118">
         <v>157182</v>
@@ -7462,13 +7462,13 @@
         <v>22</v>
       </c>
       <c r="O119" s="14" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="P119" s="14" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="Q119" s="7" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="R119">
         <v>157182</v>
@@ -7518,13 +7518,13 @@
         <v>22</v>
       </c>
       <c r="O120" s="14" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="P120" s="14" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="Q120" s="7" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="R120">
         <v>157182</v>
@@ -7574,13 +7574,13 @@
         <v>22</v>
       </c>
       <c r="O121" s="14" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="P121" s="14" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="Q121" s="7" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="R121">
         <v>157182</v>
@@ -7630,13 +7630,13 @@
         <v>22</v>
       </c>
       <c r="O122" s="14" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="P122" s="14" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="Q122" s="7" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="R122">
         <v>157182</v>
@@ -7686,13 +7686,13 @@
         <v>22</v>
       </c>
       <c r="O123" s="14" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="P123" s="14" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="Q123" s="7" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="R123">
         <v>157182</v>
@@ -7742,13 +7742,13 @@
         <v>22</v>
       </c>
       <c r="O124" s="14" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="P124" s="14" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="Q124" s="7" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="R124">
         <v>157182</v>
@@ -7798,13 +7798,13 @@
         <v>22</v>
       </c>
       <c r="O125" s="14" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="P125" s="14" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="Q125" s="7" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="R125">
         <v>157182</v>
@@ -7854,13 +7854,13 @@
         <v>22</v>
       </c>
       <c r="O126" s="14" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="P126" s="14" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="Q126" s="7" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="R126">
         <v>157182</v>
@@ -7910,13 +7910,13 @@
         <v>22</v>
       </c>
       <c r="O127" s="14" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="P127" s="14" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="Q127" s="7" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="R127">
         <v>157182</v>
@@ -7966,13 +7966,13 @@
         <v>22</v>
       </c>
       <c r="O128" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="P128" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="Q128" s="7" t="s">
         <v>93</v>
-      </c>
-      <c r="P128" s="14" t="s">
-        <v>94</v>
-      </c>
-      <c r="Q128" s="7" t="s">
-        <v>91</v>
       </c>
       <c r="R128">
         <v>157182</v>
@@ -8022,13 +8022,13 @@
         <v>22</v>
       </c>
       <c r="O129" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="P129" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="Q129" s="7" t="s">
         <v>93</v>
-      </c>
-      <c r="P129" s="14" t="s">
-        <v>94</v>
-      </c>
-      <c r="Q129" s="7" t="s">
-        <v>91</v>
       </c>
       <c r="R129">
         <v>157182</v>
@@ -8078,13 +8078,13 @@
         <v>22</v>
       </c>
       <c r="O130" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="P130" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="Q130" s="7" t="s">
         <v>93</v>
-      </c>
-      <c r="P130" s="14" t="s">
-        <v>94</v>
-      </c>
-      <c r="Q130" s="7" t="s">
-        <v>91</v>
       </c>
       <c r="R130">
         <v>157182</v>
@@ -8134,13 +8134,13 @@
         <v>22</v>
       </c>
       <c r="O131" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="P131" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="Q131" s="7" t="s">
         <v>93</v>
-      </c>
-      <c r="P131" s="14" t="s">
-        <v>94</v>
-      </c>
-      <c r="Q131" s="7" t="s">
-        <v>91</v>
       </c>
       <c r="R131">
         <v>157182</v>
@@ -8190,13 +8190,13 @@
         <v>22</v>
       </c>
       <c r="O132" s="14" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="P132" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="Q132" s="7" t="s">
         <v>94</v>
-      </c>
-      <c r="Q132" s="7" t="s">
-        <v>92</v>
       </c>
       <c r="R132">
         <v>157182</v>
@@ -8246,13 +8246,13 @@
         <v>22</v>
       </c>
       <c r="O133" s="14" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="P133" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="Q133" s="7" t="s">
         <v>94</v>
-      </c>
-      <c r="Q133" s="7" t="s">
-        <v>92</v>
       </c>
       <c r="R133">
         <v>157182</v>
@@ -8302,13 +8302,13 @@
         <v>22</v>
       </c>
       <c r="O134" s="14" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="P134" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="Q134" s="7" t="s">
         <v>94</v>
-      </c>
-      <c r="Q134" s="7" t="s">
-        <v>92</v>
       </c>
       <c r="R134">
         <v>157182</v>
@@ -8358,13 +8358,13 @@
         <v>22</v>
       </c>
       <c r="O135" s="14" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="P135" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="Q135" s="7" t="s">
         <v>94</v>
-      </c>
-      <c r="Q135" s="7" t="s">
-        <v>92</v>
       </c>
       <c r="R135">
         <v>157182</v>
@@ -8414,13 +8414,13 @@
         <v>22</v>
       </c>
       <c r="O136" s="14" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="P136" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="Q136" s="7" t="s">
         <v>94</v>
-      </c>
-      <c r="Q136" s="7" t="s">
-        <v>92</v>
       </c>
       <c r="R136">
         <v>157182</v>
@@ -8470,13 +8470,13 @@
         <v>22</v>
       </c>
       <c r="O137" s="14" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="P137" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="Q137" s="7" t="s">
         <v>94</v>
-      </c>
-      <c r="Q137" s="7" t="s">
-        <v>92</v>
       </c>
       <c r="R137">
         <v>157182</v>
@@ -8526,13 +8526,13 @@
         <v>22</v>
       </c>
       <c r="O138" s="14" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="P138" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="Q138" s="7" t="s">
         <v>94</v>
-      </c>
-      <c r="Q138" s="7" t="s">
-        <v>92</v>
       </c>
       <c r="R138">
         <v>157182</v>
@@ -8582,13 +8582,13 @@
         <v>22</v>
       </c>
       <c r="O139" s="14" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="P139" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="Q139" s="7" t="s">
         <v>94</v>
-      </c>
-      <c r="Q139" s="7" t="s">
-        <v>92</v>
       </c>
       <c r="R139">
         <v>157182</v>

</xml_diff>